<commit_message>
Has Red Train Paths in it
</commit_message>
<xml_diff>
--- a/CTC/Train Paths.xlsx
+++ b/CTC/Train Paths.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pitt-my.sharepoint.com/personal/njm130_pitt_edu/Documents/Documents/1140 Trains/trains/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Trains C\trains\CTC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{8E5114E1-DAD8-4367-BB1A-A4E00A331648}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7849A980-6B8A-46DB-8B1B-1CFF77717177}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E64775EF-75DB-4DC2-9D3A-2FF9B5C48937}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8880" xr2:uid="{49697FAA-9802-4200-863F-69C406775CAB}"/>
+    <workbookView xWindow="43095" yWindow="705" windowWidth="14610" windowHeight="15585" activeTab="1" xr2:uid="{49697FAA-9802-4200-863F-69C406775CAB}"/>
   </bookViews>
   <sheets>
     <sheet name="Green Line" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="65">
   <si>
     <t>K</t>
   </si>
@@ -197,6 +197,42 @@
   <si>
     <t>STATION; CASTLE SHANNON</t>
   </si>
+  <si>
+    <t>Red</t>
+  </si>
+  <si>
+    <t>STATION; SHADYSIDE</t>
+  </si>
+  <si>
+    <t>STATION: HERRON AVE</t>
+  </si>
+  <si>
+    <t>STATION; HERRON AVE</t>
+  </si>
+  <si>
+    <t>STATION; SWISSVILLE</t>
+  </si>
+  <si>
+    <t>UNDERGROUND</t>
+  </si>
+  <si>
+    <t>STATION; PENN STATION</t>
+  </si>
+  <si>
+    <t>STATION; STEEL PLAZA</t>
+  </si>
+  <si>
+    <t>STATION; FIRST AVE</t>
+  </si>
+  <si>
+    <t>STATION; STATION SQUARE</t>
+  </si>
+  <si>
+    <t>STATION; SOUTH HILLS JUNCTION</t>
+  </si>
+  <si>
+    <t>STATION: SHADYSIDE</t>
+  </si>
 </sst>
 </file>
 
@@ -249,7 +285,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -271,6 +307,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -608,8 +653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BC49BC8-5AFA-4F8B-8993-BD2220A0FE14}">
   <dimension ref="A1:H173"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A136" workbookViewId="0">
-      <selection activeCell="F122" sqref="F122"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -674,8 +719,8 @@
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="6">
-        <f t="shared" ref="H2:H33" si="0">D2*(1/(E2*1000/(60*60)))</f>
-        <v>6</v>
+        <f>'Red Line'!H2</f>
+        <v>6.75</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
@@ -697,7 +742,7 @@
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="H3:H33" si="0">D3*(1/(E3*1000/(60*60)))</f>
         <v>5.1428571428571432</v>
       </c>
     </row>
@@ -4755,12 +4800,2039 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{681D3D5A-AA2E-42DC-90C6-FB0A28127D18}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H106"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G97" sqref="G97"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="5" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" style="7"/>
+    <col min="4" max="4" width="7.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" style="7"/>
+    <col min="6" max="6" width="21" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.88671875" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="7">
+        <v>9</v>
+      </c>
+      <c r="D2" s="7">
+        <v>75</v>
+      </c>
+      <c r="E2" s="7">
+        <v>40</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="H2" s="7">
+        <f>D2*(1/(E2*1000/(60*60)))</f>
+        <v>6.75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="7">
+        <v>8</v>
+      </c>
+      <c r="D3" s="7">
+        <v>75</v>
+      </c>
+      <c r="E3" s="7">
+        <v>40</v>
+      </c>
+      <c r="H3" s="7">
+        <f>D3*(1/(E3*1000/(60*60)))</f>
+        <v>6.75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="7">
+        <v>7</v>
+      </c>
+      <c r="D4" s="7">
+        <v>75</v>
+      </c>
+      <c r="E4" s="7">
+        <v>40</v>
+      </c>
+      <c r="F4" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" s="7">
+        <f t="shared" ref="H4" si="0">D4*(1/(E4*1000/(60*60)))</f>
+        <v>6.75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="7">
+        <v>6</v>
+      </c>
+      <c r="D5" s="7">
+        <v>50</v>
+      </c>
+      <c r="E5" s="7">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="7">
+        <v>5</v>
+      </c>
+      <c r="D6" s="7">
+        <v>50</v>
+      </c>
+      <c r="E6" s="7">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="7">
+        <v>4</v>
+      </c>
+      <c r="D7" s="7">
+        <v>50</v>
+      </c>
+      <c r="E7" s="7">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="7">
+        <v>3</v>
+      </c>
+      <c r="D8" s="7">
+        <v>50</v>
+      </c>
+      <c r="E8" s="7">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="7">
+        <v>2</v>
+      </c>
+      <c r="D9" s="7">
+        <v>50</v>
+      </c>
+      <c r="E9" s="7">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="7">
+        <v>1</v>
+      </c>
+      <c r="D10" s="7">
+        <v>50</v>
+      </c>
+      <c r="E10" s="7">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="8">
+        <v>16</v>
+      </c>
+      <c r="D11" s="8">
+        <v>50</v>
+      </c>
+      <c r="E11" s="8">
+        <v>40</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="10">
+        <v>17</v>
+      </c>
+      <c r="D12" s="8">
+        <v>200</v>
+      </c>
+      <c r="E12" s="8">
+        <v>55</v>
+      </c>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+    </row>
+    <row r="13" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="8">
+        <v>18</v>
+      </c>
+      <c r="D13" s="8">
+        <v>400</v>
+      </c>
+      <c r="E13" s="8">
+        <v>70</v>
+      </c>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+    </row>
+    <row r="14" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="8">
+        <v>19</v>
+      </c>
+      <c r="D14" s="8">
+        <v>400</v>
+      </c>
+      <c r="E14" s="8">
+        <v>70</v>
+      </c>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+    </row>
+    <row r="15" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="10">
+        <v>20</v>
+      </c>
+      <c r="D15" s="8">
+        <v>200</v>
+      </c>
+      <c r="E15" s="8">
+        <v>70</v>
+      </c>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+    </row>
+    <row r="16" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="8">
+        <v>21</v>
+      </c>
+      <c r="D16" s="8">
+        <v>100</v>
+      </c>
+      <c r="E16" s="8">
+        <v>55</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" s="10">
+        <v>22</v>
+      </c>
+      <c r="D17" s="8">
+        <v>100</v>
+      </c>
+      <c r="E17" s="8">
+        <v>55</v>
+      </c>
+      <c r="F17" s="8"/>
+    </row>
+    <row r="18" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="8">
+        <v>23</v>
+      </c>
+      <c r="D18" s="8">
+        <v>100</v>
+      </c>
+      <c r="E18" s="8">
+        <v>55</v>
+      </c>
+      <c r="F18" s="8"/>
+    </row>
+    <row r="19" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="8">
+        <v>24</v>
+      </c>
+      <c r="D19" s="8">
+        <v>50</v>
+      </c>
+      <c r="E19" s="8">
+        <v>70</v>
+      </c>
+      <c r="F19" s="8"/>
+    </row>
+    <row r="20" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A20" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="10">
+        <v>25</v>
+      </c>
+      <c r="D20" s="8">
+        <v>50</v>
+      </c>
+      <c r="E20" s="8">
+        <v>70</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="8">
+        <v>26</v>
+      </c>
+      <c r="D21" s="8">
+        <v>50</v>
+      </c>
+      <c r="E21" s="8">
+        <v>70</v>
+      </c>
+      <c r="F21" s="8"/>
+    </row>
+    <row r="22" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="10">
+        <v>27</v>
+      </c>
+      <c r="D22" s="8">
+        <v>50</v>
+      </c>
+      <c r="E22" s="8">
+        <v>70</v>
+      </c>
+      <c r="F22" s="9"/>
+    </row>
+    <row r="23" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A23" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" s="8">
+        <v>28</v>
+      </c>
+      <c r="D23" s="8">
+        <v>50</v>
+      </c>
+      <c r="E23" s="8">
+        <v>70</v>
+      </c>
+      <c r="F23" s="8"/>
+    </row>
+    <row r="24" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A24" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C24" s="8">
+        <v>29</v>
+      </c>
+      <c r="D24" s="8">
+        <v>60</v>
+      </c>
+      <c r="E24" s="8">
+        <v>70</v>
+      </c>
+      <c r="F24" s="8"/>
+    </row>
+    <row r="25" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" s="10">
+        <v>30</v>
+      </c>
+      <c r="D25" s="8">
+        <v>60</v>
+      </c>
+      <c r="E25" s="8">
+        <v>70</v>
+      </c>
+      <c r="F25" s="8"/>
+    </row>
+    <row r="26" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26" s="8">
+        <v>31</v>
+      </c>
+      <c r="D26" s="8">
+        <v>50</v>
+      </c>
+      <c r="E26" s="8">
+        <v>70</v>
+      </c>
+      <c r="F26" s="8"/>
+    </row>
+    <row r="27" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C27" s="10">
+        <v>32</v>
+      </c>
+      <c r="D27" s="8">
+        <v>50</v>
+      </c>
+      <c r="E27" s="8">
+        <v>70</v>
+      </c>
+      <c r="F27" s="9"/>
+    </row>
+    <row r="28" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C28" s="8">
+        <v>33</v>
+      </c>
+      <c r="D28" s="8">
+        <v>50</v>
+      </c>
+      <c r="E28" s="8">
+        <v>70</v>
+      </c>
+      <c r="F28" s="8"/>
+    </row>
+    <row r="29" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C29" s="8">
+        <v>34</v>
+      </c>
+      <c r="D29" s="8">
+        <v>50</v>
+      </c>
+      <c r="E29" s="8">
+        <v>70</v>
+      </c>
+      <c r="F29" s="8"/>
+    </row>
+    <row r="30" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A30" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C30" s="10">
+        <v>35</v>
+      </c>
+      <c r="D30" s="8">
+        <v>50</v>
+      </c>
+      <c r="E30" s="8">
+        <v>70</v>
+      </c>
+      <c r="F30" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A31" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C31" s="8">
+        <v>36</v>
+      </c>
+      <c r="D31" s="8">
+        <v>50</v>
+      </c>
+      <c r="E31" s="8">
+        <v>70</v>
+      </c>
+      <c r="F31" s="8"/>
+    </row>
+    <row r="32" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A32" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C32" s="8">
+        <v>37</v>
+      </c>
+      <c r="D32" s="8">
+        <v>50</v>
+      </c>
+      <c r="E32" s="8">
+        <v>70</v>
+      </c>
+      <c r="F32" s="8"/>
+    </row>
+    <row r="33" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A33" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C33" s="10">
+        <v>38</v>
+      </c>
+      <c r="D33" s="8">
+        <v>50</v>
+      </c>
+      <c r="E33" s="8">
+        <v>70</v>
+      </c>
+      <c r="F33" s="9"/>
+    </row>
+    <row r="34" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A34" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C34" s="8">
+        <v>39</v>
+      </c>
+      <c r="D34" s="8">
+        <v>50</v>
+      </c>
+      <c r="E34" s="8">
+        <v>70</v>
+      </c>
+      <c r="F34" s="8"/>
+    </row>
+    <row r="35" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A35" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C35" s="8">
+        <v>40</v>
+      </c>
+      <c r="D35" s="8">
+        <v>60</v>
+      </c>
+      <c r="E35" s="8">
+        <v>70</v>
+      </c>
+      <c r="F35" s="8"/>
+    </row>
+    <row r="36" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A36" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C36" s="10">
+        <v>41</v>
+      </c>
+      <c r="D36" s="8">
+        <v>60</v>
+      </c>
+      <c r="E36" s="8">
+        <v>70</v>
+      </c>
+      <c r="F36" s="8"/>
+    </row>
+    <row r="37" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A37" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C37" s="8">
+        <v>42</v>
+      </c>
+      <c r="D37" s="8">
+        <v>50</v>
+      </c>
+      <c r="E37" s="8">
+        <v>70</v>
+      </c>
+      <c r="F37" s="8"/>
+    </row>
+    <row r="38" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A38" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C38" s="8">
+        <v>43</v>
+      </c>
+      <c r="D38" s="8">
+        <v>50</v>
+      </c>
+      <c r="E38" s="8">
+        <v>70</v>
+      </c>
+      <c r="F38" s="9"/>
+    </row>
+    <row r="39" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A39" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C39" s="10">
+        <v>44</v>
+      </c>
+      <c r="D39" s="8">
+        <v>50</v>
+      </c>
+      <c r="E39" s="8">
+        <v>70</v>
+      </c>
+      <c r="F39" s="8"/>
+    </row>
+    <row r="40" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A40" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C40" s="8">
+        <v>45</v>
+      </c>
+      <c r="D40" s="8">
+        <v>50</v>
+      </c>
+      <c r="E40" s="8">
+        <v>70</v>
+      </c>
+      <c r="F40" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="G40" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A41" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C41" s="8">
+        <v>46</v>
+      </c>
+      <c r="D41" s="8">
+        <v>75</v>
+      </c>
+      <c r="E41" s="8">
+        <v>70</v>
+      </c>
+      <c r="F41" s="8"/>
+    </row>
+    <row r="42" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A42" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C42" s="10">
+        <v>47</v>
+      </c>
+      <c r="D42" s="8">
+        <v>75</v>
+      </c>
+      <c r="E42" s="8">
+        <v>70</v>
+      </c>
+      <c r="F42" s="9"/>
+    </row>
+    <row r="43" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A43" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C43" s="8">
+        <v>48</v>
+      </c>
+      <c r="D43" s="8">
+        <v>75</v>
+      </c>
+      <c r="E43" s="8">
+        <v>70</v>
+      </c>
+      <c r="F43" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="G43" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A44" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C44" s="8">
+        <v>49</v>
+      </c>
+      <c r="D44" s="8">
+        <v>50</v>
+      </c>
+      <c r="E44" s="8">
+        <v>60</v>
+      </c>
+      <c r="F44" s="8"/>
+    </row>
+    <row r="45" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A45" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C45" s="10">
+        <v>50</v>
+      </c>
+      <c r="D45" s="8">
+        <v>50</v>
+      </c>
+      <c r="E45" s="8">
+        <v>60</v>
+      </c>
+      <c r="F45" s="8"/>
+    </row>
+    <row r="46" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A46" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C46" s="8">
+        <v>51</v>
+      </c>
+      <c r="D46" s="8">
+        <v>50</v>
+      </c>
+      <c r="E46" s="8">
+        <v>55</v>
+      </c>
+      <c r="F46" s="8"/>
+    </row>
+    <row r="47" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A47" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C47" s="8">
+        <v>52</v>
+      </c>
+      <c r="D47" s="8">
+        <v>43.2</v>
+      </c>
+      <c r="E47" s="8">
+        <v>55</v>
+      </c>
+      <c r="F47" s="8"/>
+    </row>
+    <row r="48" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A48" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C48" s="10">
+        <v>53</v>
+      </c>
+      <c r="D48" s="8">
+        <v>50</v>
+      </c>
+      <c r="E48" s="8">
+        <v>55</v>
+      </c>
+      <c r="F48" s="8"/>
+    </row>
+    <row r="49" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A49" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C49" s="8">
+        <v>54</v>
+      </c>
+      <c r="D49" s="8">
+        <v>50</v>
+      </c>
+      <c r="E49" s="8">
+        <v>55</v>
+      </c>
+      <c r="F49" s="8"/>
+    </row>
+    <row r="50" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A50" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C50" s="8">
+        <v>55</v>
+      </c>
+      <c r="D50" s="8">
+        <v>75</v>
+      </c>
+      <c r="E50" s="8">
+        <v>55</v>
+      </c>
+      <c r="F50" s="8"/>
+    </row>
+    <row r="51" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A51" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C51" s="10">
+        <v>56</v>
+      </c>
+      <c r="D51" s="8">
+        <v>75</v>
+      </c>
+      <c r="E51" s="8">
+        <v>55</v>
+      </c>
+      <c r="F51" s="8"/>
+    </row>
+    <row r="52" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A52" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C52" s="8">
+        <v>57</v>
+      </c>
+      <c r="D52" s="8">
+        <v>75</v>
+      </c>
+      <c r="E52" s="8">
+        <v>55</v>
+      </c>
+      <c r="F52" s="8"/>
+    </row>
+    <row r="53" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A53" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C53" s="8">
+        <v>58</v>
+      </c>
+      <c r="D53" s="8">
+        <v>75</v>
+      </c>
+      <c r="E53" s="8">
+        <v>55</v>
+      </c>
+      <c r="F53" s="8"/>
+    </row>
+    <row r="54" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A54" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C54" s="10">
+        <v>59</v>
+      </c>
+      <c r="D54" s="8">
+        <v>75</v>
+      </c>
+      <c r="E54" s="8">
+        <v>55</v>
+      </c>
+      <c r="F54" s="8"/>
+    </row>
+    <row r="55" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A55" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B55" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C55" s="8">
+        <v>60</v>
+      </c>
+      <c r="D55" s="8">
+        <v>75</v>
+      </c>
+      <c r="E55" s="8">
+        <v>55</v>
+      </c>
+      <c r="F55" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="G55" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A56" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B56" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C56" s="8">
+        <v>61</v>
+      </c>
+      <c r="D56" s="8">
+        <v>75</v>
+      </c>
+      <c r="E56" s="8">
+        <v>55</v>
+      </c>
+      <c r="F56" s="8"/>
+    </row>
+    <row r="57" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A57" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B57" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C57" s="10">
+        <v>62</v>
+      </c>
+      <c r="D57" s="8">
+        <v>75</v>
+      </c>
+      <c r="E57" s="8">
+        <v>55</v>
+      </c>
+      <c r="F57" s="8"/>
+    </row>
+    <row r="58" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A58" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B58" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C58" s="8">
+        <v>63</v>
+      </c>
+      <c r="D58" s="8">
+        <v>75</v>
+      </c>
+      <c r="E58" s="8">
+        <v>55</v>
+      </c>
+      <c r="F58" s="8"/>
+    </row>
+    <row r="59" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A59" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B59" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C59" s="8">
+        <v>64</v>
+      </c>
+      <c r="D59" s="8">
+        <v>75</v>
+      </c>
+      <c r="E59" s="8">
+        <v>55</v>
+      </c>
+      <c r="F59" s="8"/>
+    </row>
+    <row r="60" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A60" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B60" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C60" s="10">
+        <v>65</v>
+      </c>
+      <c r="D60" s="8">
+        <v>75</v>
+      </c>
+      <c r="E60" s="8">
+        <v>55</v>
+      </c>
+      <c r="F60" s="8"/>
+    </row>
+    <row r="61" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A61" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B61" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C61" s="8">
+        <v>66</v>
+      </c>
+      <c r="D61" s="8">
+        <v>75</v>
+      </c>
+      <c r="E61" s="8">
+        <v>55</v>
+      </c>
+      <c r="F61" s="8"/>
+    </row>
+    <row r="62" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A62" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B62" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C62" s="8">
+        <v>52</v>
+      </c>
+      <c r="D62" s="8">
+        <v>43.2</v>
+      </c>
+      <c r="E62" s="8">
+        <v>55</v>
+      </c>
+      <c r="F62" s="8"/>
+    </row>
+    <row r="63" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A63" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B63" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C63" s="8">
+        <v>51</v>
+      </c>
+      <c r="D63" s="8">
+        <v>50</v>
+      </c>
+      <c r="E63" s="8">
+        <v>55</v>
+      </c>
+      <c r="F63" s="8"/>
+    </row>
+    <row r="64" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A64" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B64" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C64" s="10">
+        <v>50</v>
+      </c>
+      <c r="D64" s="8">
+        <v>50</v>
+      </c>
+      <c r="E64" s="8">
+        <v>60</v>
+      </c>
+      <c r="F64" s="8"/>
+    </row>
+    <row r="65" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A65" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B65" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C65" s="8">
+        <v>49</v>
+      </c>
+      <c r="D65" s="8">
+        <v>50</v>
+      </c>
+      <c r="E65" s="8">
+        <v>60</v>
+      </c>
+      <c r="F65" s="8"/>
+    </row>
+    <row r="66" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A66" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B66" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C66" s="8">
+        <v>48</v>
+      </c>
+      <c r="D66" s="8">
+        <v>75</v>
+      </c>
+      <c r="E66" s="8">
+        <v>70</v>
+      </c>
+      <c r="F66" s="9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A67" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B67" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C67" s="10">
+        <v>47</v>
+      </c>
+      <c r="D67" s="8">
+        <v>75</v>
+      </c>
+      <c r="E67" s="8">
+        <v>70</v>
+      </c>
+      <c r="F67" s="9"/>
+    </row>
+    <row r="68" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A68" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B68" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C68" s="8">
+        <v>46</v>
+      </c>
+      <c r="D68" s="8">
+        <v>75</v>
+      </c>
+      <c r="E68" s="8">
+        <v>70</v>
+      </c>
+      <c r="F68" s="8"/>
+    </row>
+    <row r="69" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A69" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B69" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C69" s="8">
+        <v>45</v>
+      </c>
+      <c r="D69" s="8">
+        <v>50</v>
+      </c>
+      <c r="E69" s="8">
+        <v>70</v>
+      </c>
+      <c r="F69" s="9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A70" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B70" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C70" s="10">
+        <v>44</v>
+      </c>
+      <c r="D70" s="8">
+        <v>50</v>
+      </c>
+      <c r="E70" s="8">
+        <v>70</v>
+      </c>
+      <c r="F70" s="8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A71" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B71" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C71" s="8">
+        <v>67</v>
+      </c>
+      <c r="D71" s="8">
+        <v>50</v>
+      </c>
+      <c r="E71" s="8">
+        <v>55</v>
+      </c>
+      <c r="F71" s="8"/>
+    </row>
+    <row r="72" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A72" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B72" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C72" s="10">
+        <v>68</v>
+      </c>
+      <c r="D72" s="8">
+        <v>50</v>
+      </c>
+      <c r="E72" s="8">
+        <v>55</v>
+      </c>
+      <c r="F72" s="8"/>
+    </row>
+    <row r="73" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A73" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B73" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C73" s="8">
+        <v>69</v>
+      </c>
+      <c r="D73" s="8">
+        <v>50</v>
+      </c>
+      <c r="E73" s="8">
+        <v>55</v>
+      </c>
+      <c r="F73" s="8"/>
+    </row>
+    <row r="74" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A74" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B74" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C74" s="8">
+        <v>70</v>
+      </c>
+      <c r="D74" s="8">
+        <v>50</v>
+      </c>
+      <c r="E74" s="8">
+        <v>55</v>
+      </c>
+      <c r="F74" s="8"/>
+    </row>
+    <row r="75" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A75" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B75" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C75" s="10">
+        <v>71</v>
+      </c>
+      <c r="D75" s="8">
+        <v>50</v>
+      </c>
+      <c r="E75" s="8">
+        <v>55</v>
+      </c>
+      <c r="F75" s="8"/>
+    </row>
+    <row r="76" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A76" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B76" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C76" s="10">
+        <v>38</v>
+      </c>
+      <c r="D76" s="8">
+        <v>50</v>
+      </c>
+      <c r="E76" s="8">
+        <v>70</v>
+      </c>
+      <c r="F76" s="9"/>
+    </row>
+    <row r="77" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A77" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B77" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C77" s="8">
+        <v>37</v>
+      </c>
+      <c r="D77" s="8">
+        <v>50</v>
+      </c>
+      <c r="E77" s="8">
+        <v>70</v>
+      </c>
+      <c r="F77" s="8"/>
+    </row>
+    <row r="78" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A78" s="8" t="str">
+        <f t="shared" ref="A78:A98" si="1">A77</f>
+        <v>Red</v>
+      </c>
+      <c r="B78" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C78" s="8">
+        <v>36</v>
+      </c>
+      <c r="D78" s="8">
+        <v>50</v>
+      </c>
+      <c r="E78" s="8">
+        <v>70</v>
+      </c>
+      <c r="F78" s="8"/>
+    </row>
+    <row r="79" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A79" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>Red</v>
+      </c>
+      <c r="B79" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C79" s="10">
+        <v>35</v>
+      </c>
+      <c r="D79" s="8">
+        <v>50</v>
+      </c>
+      <c r="E79" s="8">
+        <v>70</v>
+      </c>
+      <c r="F79" s="9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A80" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>Red</v>
+      </c>
+      <c r="B80" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C80" s="8">
+        <v>34</v>
+      </c>
+      <c r="D80" s="8">
+        <v>50</v>
+      </c>
+      <c r="E80" s="8">
+        <v>70</v>
+      </c>
+      <c r="F80" s="8"/>
+    </row>
+    <row r="81" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A81" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>Red</v>
+      </c>
+      <c r="B81" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C81" s="8">
+        <v>33</v>
+      </c>
+      <c r="D81" s="8">
+        <v>50</v>
+      </c>
+      <c r="E81" s="8">
+        <v>70</v>
+      </c>
+      <c r="F81" s="8"/>
+    </row>
+    <row r="82" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A82" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>Red</v>
+      </c>
+      <c r="B82" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C82" s="8">
+        <v>72</v>
+      </c>
+      <c r="D82" s="8">
+        <v>50</v>
+      </c>
+      <c r="E82" s="8">
+        <v>55</v>
+      </c>
+      <c r="F82" s="8"/>
+    </row>
+    <row r="83" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A83" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>Red</v>
+      </c>
+      <c r="B83" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C83" s="8">
+        <v>73</v>
+      </c>
+      <c r="D83" s="8">
+        <v>50</v>
+      </c>
+      <c r="E83" s="8">
+        <v>55</v>
+      </c>
+      <c r="F83" s="8"/>
+    </row>
+    <row r="84" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A84" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>Red</v>
+      </c>
+      <c r="B84" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C84" s="10">
+        <v>74</v>
+      </c>
+      <c r="D84" s="8">
+        <v>50</v>
+      </c>
+      <c r="E84" s="8">
+        <v>55</v>
+      </c>
+      <c r="F84" s="8"/>
+    </row>
+    <row r="85" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A85" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>Red</v>
+      </c>
+      <c r="B85" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C85" s="8">
+        <v>75</v>
+      </c>
+      <c r="D85" s="8">
+        <v>50</v>
+      </c>
+      <c r="E85" s="8">
+        <v>55</v>
+      </c>
+      <c r="F85" s="8"/>
+    </row>
+    <row r="86" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A86" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>Red</v>
+      </c>
+      <c r="B86" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C86" s="8">
+        <v>76</v>
+      </c>
+      <c r="D86" s="8">
+        <v>50</v>
+      </c>
+      <c r="E86" s="8">
+        <v>55</v>
+      </c>
+      <c r="F86" s="8"/>
+    </row>
+    <row r="87" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A87" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>Red</v>
+      </c>
+      <c r="B87" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C87" s="10">
+        <v>27</v>
+      </c>
+      <c r="D87" s="8">
+        <v>50</v>
+      </c>
+      <c r="E87" s="8">
+        <v>70</v>
+      </c>
+      <c r="F87" s="9"/>
+    </row>
+    <row r="88" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A88" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>Red</v>
+      </c>
+      <c r="B88" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C88" s="8">
+        <v>26</v>
+      </c>
+      <c r="D88" s="8">
+        <v>50</v>
+      </c>
+      <c r="E88" s="8">
+        <v>70</v>
+      </c>
+      <c r="F88" s="8"/>
+    </row>
+    <row r="89" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A89" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>Red</v>
+      </c>
+      <c r="B89" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C89" s="10">
+        <v>25</v>
+      </c>
+      <c r="D89" s="8">
+        <v>50</v>
+      </c>
+      <c r="E89" s="8">
+        <v>70</v>
+      </c>
+      <c r="F89" s="9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A90" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>Red</v>
+      </c>
+      <c r="B90" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C90" s="8">
+        <v>24</v>
+      </c>
+      <c r="D90" s="8">
+        <v>50</v>
+      </c>
+      <c r="E90" s="8">
+        <v>70</v>
+      </c>
+      <c r="F90" s="8"/>
+    </row>
+    <row r="91" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A91" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>Red</v>
+      </c>
+      <c r="B91" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C91" s="8">
+        <v>23</v>
+      </c>
+      <c r="D91" s="8">
+        <v>100</v>
+      </c>
+      <c r="E91" s="8">
+        <v>55</v>
+      </c>
+      <c r="F91" s="8"/>
+    </row>
+    <row r="92" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A92" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>Red</v>
+      </c>
+      <c r="B92" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C92" s="10">
+        <v>22</v>
+      </c>
+      <c r="D92" s="8">
+        <v>100</v>
+      </c>
+      <c r="E92" s="8">
+        <v>55</v>
+      </c>
+      <c r="F92" s="8"/>
+    </row>
+    <row r="93" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A93" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>Red</v>
+      </c>
+      <c r="B93" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C93" s="8">
+        <v>21</v>
+      </c>
+      <c r="D93" s="8">
+        <v>100</v>
+      </c>
+      <c r="E93" s="8">
+        <v>55</v>
+      </c>
+      <c r="F93" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A94" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>Red</v>
+      </c>
+      <c r="B94" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C94" s="10">
+        <v>20</v>
+      </c>
+      <c r="D94" s="8">
+        <v>200</v>
+      </c>
+      <c r="E94" s="8">
+        <v>70</v>
+      </c>
+      <c r="F94" s="8"/>
+    </row>
+    <row r="95" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A95" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>Red</v>
+      </c>
+      <c r="B95" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C95" s="8">
+        <v>19</v>
+      </c>
+      <c r="D95" s="8">
+        <v>400</v>
+      </c>
+      <c r="E95" s="8">
+        <v>70</v>
+      </c>
+      <c r="F95" s="8"/>
+    </row>
+    <row r="96" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A96" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>Red</v>
+      </c>
+      <c r="B96" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C96" s="8">
+        <v>18</v>
+      </c>
+      <c r="D96" s="8">
+        <v>400</v>
+      </c>
+      <c r="E96" s="8">
+        <v>70</v>
+      </c>
+      <c r="F96" s="8"/>
+    </row>
+    <row r="97" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A97" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>Red</v>
+      </c>
+      <c r="B97" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C97" s="10">
+        <v>17</v>
+      </c>
+      <c r="D97" s="8">
+        <v>200</v>
+      </c>
+      <c r="E97" s="8">
+        <v>55</v>
+      </c>
+      <c r="F97" s="8"/>
+    </row>
+    <row r="98" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A98" s="8" t="str">
+        <f t="shared" si="1"/>
+        <v>Red</v>
+      </c>
+      <c r="B98" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C98" s="8">
+        <v>16</v>
+      </c>
+      <c r="D98" s="8">
+        <v>50</v>
+      </c>
+      <c r="E98" s="8">
+        <v>40</v>
+      </c>
+      <c r="F98" s="9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A99" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B99" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C99" s="10">
+        <v>1</v>
+      </c>
+      <c r="D99" s="8">
+        <v>50</v>
+      </c>
+      <c r="E99" s="8">
+        <v>40</v>
+      </c>
+      <c r="F99" s="8"/>
+    </row>
+    <row r="100" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A100" s="8" t="str">
+        <f>A99</f>
+        <v>Red</v>
+      </c>
+      <c r="B100" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C100" s="8">
+        <v>2</v>
+      </c>
+      <c r="D100" s="8">
+        <v>50</v>
+      </c>
+      <c r="E100" s="8">
+        <v>40</v>
+      </c>
+      <c r="F100" s="8"/>
+    </row>
+    <row r="101" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A101" s="8" t="str">
+        <f t="shared" ref="A101:A106" si="2">A100</f>
+        <v>Red</v>
+      </c>
+      <c r="B101" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C101" s="8">
+        <v>3</v>
+      </c>
+      <c r="D101" s="8">
+        <v>50</v>
+      </c>
+      <c r="E101" s="8">
+        <v>40</v>
+      </c>
+      <c r="F101" s="8"/>
+    </row>
+    <row r="102" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A102" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>Red</v>
+      </c>
+      <c r="B102" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C102" s="10">
+        <v>4</v>
+      </c>
+      <c r="D102" s="8">
+        <v>50</v>
+      </c>
+      <c r="E102" s="8">
+        <v>40</v>
+      </c>
+      <c r="F102" s="8"/>
+    </row>
+    <row r="103" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A103" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>Red</v>
+      </c>
+      <c r="B103" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C103" s="8">
+        <v>5</v>
+      </c>
+      <c r="D103" s="8">
+        <v>50</v>
+      </c>
+      <c r="E103" s="8">
+        <v>40</v>
+      </c>
+      <c r="F103" s="8"/>
+    </row>
+    <row r="104" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A104" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>Red</v>
+      </c>
+      <c r="B104" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C104" s="8">
+        <v>6</v>
+      </c>
+      <c r="D104" s="8">
+        <v>50</v>
+      </c>
+      <c r="E104" s="8">
+        <v>40</v>
+      </c>
+      <c r="F104" s="8"/>
+    </row>
+    <row r="105" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A105" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>Red</v>
+      </c>
+      <c r="B105" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C105" s="10">
+        <v>7</v>
+      </c>
+      <c r="D105" s="8">
+        <v>75</v>
+      </c>
+      <c r="E105" s="8">
+        <v>40</v>
+      </c>
+      <c r="F105" s="9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A106" s="8" t="str">
+        <f t="shared" si="2"/>
+        <v>Red</v>
+      </c>
+      <c r="B106" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C106" s="8">
+        <v>8</v>
+      </c>
+      <c r="D106" s="8">
+        <v>75</v>
+      </c>
+      <c r="E106" s="8">
+        <v>40</v>
+      </c>
+      <c r="F106" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
inbound and outbound stations
</commit_message>
<xml_diff>
--- a/CTC/Train Paths.xlsx
+++ b/CTC/Train Paths.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Trains C\trains\CTC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E64775EF-75DB-4DC2-9D3A-2FF9B5C48937}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FB86ABF-76A6-4D61-9482-9FC0B2A13C8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43095" yWindow="705" windowWidth="14610" windowHeight="15585" activeTab="1" xr2:uid="{49697FAA-9802-4200-863F-69C406775CAB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{49697FAA-9802-4200-863F-69C406775CAB}"/>
   </bookViews>
   <sheets>
     <sheet name="Green Line" sheetId="2" r:id="rId1"/>
@@ -37,14 +37,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="70">
   <si>
     <t>K</t>
   </si>
   <si>
-    <t>STATION; GLENBURY</t>
-  </si>
-  <si>
     <t>Right</t>
   </si>
   <si>
@@ -75,9 +72,6 @@
     <t>L</t>
   </si>
   <si>
-    <t>STATION; DORMONT</t>
-  </si>
-  <si>
     <t>M</t>
   </si>
   <si>
@@ -177,15 +171,6 @@
     <t>J</t>
   </si>
   <si>
-    <t>STATION; OVERBROOK</t>
-  </si>
-  <si>
-    <t>STATION; INGLEWOOD</t>
-  </si>
-  <si>
-    <t>STATION; CENTRAL</t>
-  </si>
-  <si>
     <t>STATION; LEBRON</t>
   </si>
   <si>
@@ -232,6 +217,36 @@
   </si>
   <si>
     <t>STATION: SHADYSIDE</t>
+  </si>
+  <si>
+    <t>STATION; GLENBURY OUT</t>
+  </si>
+  <si>
+    <t>STATION; DORMONT OUT</t>
+  </si>
+  <si>
+    <t>STATION; DORMONT IN</t>
+  </si>
+  <si>
+    <t>STATION; GLENBURY IN</t>
+  </si>
+  <si>
+    <t>STATION; OVERBROOK OUT</t>
+  </si>
+  <si>
+    <t>STATION; INGLEWOOD OUT</t>
+  </si>
+  <si>
+    <t>STATION; CENTRAL OUT</t>
+  </si>
+  <si>
+    <t>STATION; CENTRAL IN</t>
+  </si>
+  <si>
+    <t>STATION; INGLEWOOD IN</t>
+  </si>
+  <si>
+    <t>STATION; OVERBROOK IN</t>
   </si>
 </sst>
 </file>
@@ -653,8 +668,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BC49BC8-5AFA-4F8B-8993-BD2220A0FE14}">
   <dimension ref="A1:H173"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="A156" workbookViewId="0">
+      <selection activeCell="F167" sqref="F167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -674,36 +689,36 @@
   <sheetData>
     <row r="1" spans="1:8" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C2" s="4">
         <v>62</v>
@@ -715,7 +730,7 @@
         <v>30</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="6">
@@ -725,7 +740,7 @@
     </row>
     <row r="3" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>0</v>
@@ -748,7 +763,7 @@
     </row>
     <row r="4" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>0</v>
@@ -771,7 +786,7 @@
     </row>
     <row r="5" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>0</v>
@@ -786,10 +801,10 @@
         <v>70</v>
       </c>
       <c r="F5" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>1</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>2</v>
       </c>
       <c r="H5" s="6">
         <f t="shared" si="0"/>
@@ -798,7 +813,7 @@
     </row>
     <row r="6" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>0</v>
@@ -821,7 +836,7 @@
     </row>
     <row r="7" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>0</v>
@@ -844,7 +859,7 @@
     </row>
     <row r="8" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>0</v>
@@ -867,10 +882,10 @@
     </row>
     <row r="9" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9" s="3">
         <v>69</v>
@@ -890,10 +905,10 @@
     </row>
     <row r="10" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C10" s="3">
         <v>70</v>
@@ -913,10 +928,10 @@
     </row>
     <row r="11" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C11" s="4">
         <v>71</v>
@@ -936,10 +951,10 @@
     </row>
     <row r="12" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12" s="3">
         <v>72</v>
@@ -959,10 +974,10 @@
     </row>
     <row r="13" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C13" s="3">
         <v>73</v>
@@ -974,10 +989,10 @@
         <v>40</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>12</v>
+        <v>61</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H13" s="6">
         <f t="shared" si="0"/>
@@ -986,10 +1001,10 @@
     </row>
     <row r="14" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C14" s="4">
         <v>74</v>
@@ -1009,10 +1024,10 @@
     </row>
     <row r="15" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C15" s="3">
         <v>75</v>
@@ -1032,10 +1047,10 @@
     </row>
     <row r="16" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C16" s="3">
         <v>76</v>
@@ -1055,10 +1070,10 @@
     </row>
     <row r="17" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C17" s="3">
         <v>77</v>
@@ -1070,10 +1085,10 @@
         <v>70</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H17" s="6">
         <f t="shared" si="0"/>
@@ -1082,10 +1097,10 @@
     </row>
     <row r="18" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C18" s="4">
         <v>78</v>
@@ -1105,10 +1120,10 @@
     </row>
     <row r="19" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C19" s="3">
         <v>79</v>
@@ -1128,10 +1143,10 @@
     </row>
     <row r="20" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C20" s="3">
         <v>80</v>
@@ -1151,10 +1166,10 @@
     </row>
     <row r="21" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C21" s="3">
         <v>81</v>
@@ -1174,10 +1189,10 @@
     </row>
     <row r="22" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C22" s="4">
         <v>82</v>
@@ -1197,10 +1212,10 @@
     </row>
     <row r="23" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C23" s="3">
         <v>83</v>
@@ -1220,10 +1235,10 @@
     </row>
     <row r="24" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C24" s="3">
         <v>84</v>
@@ -1243,10 +1258,10 @@
     </row>
     <row r="25" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C25" s="3">
         <v>85</v>
@@ -1266,10 +1281,10 @@
     </row>
     <row r="26" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C26" s="4">
         <v>86</v>
@@ -1289,10 +1304,10 @@
     </row>
     <row r="27" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C27" s="3">
         <v>87</v>
@@ -1312,10 +1327,10 @@
     </row>
     <row r="28" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C28" s="3">
         <v>88</v>
@@ -1327,10 +1342,10 @@
         <v>25</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H28" s="6">
         <f t="shared" si="0"/>
@@ -1339,10 +1354,10 @@
     </row>
     <row r="29" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C29" s="3">
         <v>89</v>
@@ -1362,10 +1377,10 @@
     </row>
     <row r="30" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C30" s="4">
         <v>90</v>
@@ -1385,10 +1400,10 @@
     </row>
     <row r="31" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C31" s="3">
         <v>91</v>
@@ -1408,10 +1423,10 @@
     </row>
     <row r="32" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C32" s="3">
         <v>92</v>
@@ -1431,10 +1446,10 @@
     </row>
     <row r="33" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C33" s="3">
         <v>93</v>
@@ -1454,10 +1469,10 @@
     </row>
     <row r="34" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C34" s="4">
         <v>94</v>
@@ -1477,10 +1492,10 @@
     </row>
     <row r="35" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C35" s="3">
         <v>95</v>
@@ -1500,10 +1515,10 @@
     </row>
     <row r="36" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C36" s="3">
         <v>96</v>
@@ -1515,10 +1530,10 @@
         <v>25</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H36" s="6">
         <f t="shared" si="1"/>
@@ -1527,10 +1542,10 @@
     </row>
     <row r="37" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C37" s="3">
         <v>97</v>
@@ -1550,10 +1565,10 @@
     </row>
     <row r="38" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C38" s="4">
         <v>98</v>
@@ -1573,10 +1588,10 @@
     </row>
     <row r="39" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C39" s="3">
         <v>99</v>
@@ -1596,10 +1611,10 @@
     </row>
     <row r="40" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C40" s="3">
         <v>100</v>
@@ -1619,10 +1634,10 @@
     </row>
     <row r="41" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C41" s="3">
         <v>85</v>
@@ -1642,10 +1657,10 @@
     </row>
     <row r="42" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C42" s="3">
         <v>84</v>
@@ -1665,10 +1680,10 @@
     </row>
     <row r="43" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C43" s="3">
         <v>83</v>
@@ -1688,10 +1703,10 @@
     </row>
     <row r="44" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C44" s="4">
         <v>82</v>
@@ -1711,10 +1726,10 @@
     </row>
     <row r="45" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C45" s="3">
         <v>81</v>
@@ -1734,10 +1749,10 @@
     </row>
     <row r="46" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C46" s="3">
         <v>80</v>
@@ -1757,10 +1772,10 @@
     </row>
     <row r="47" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C47" s="3">
         <v>79</v>
@@ -1780,10 +1795,10 @@
     </row>
     <row r="48" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C48" s="4">
         <v>78</v>
@@ -1803,10 +1818,10 @@
     </row>
     <row r="49" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C49" s="3">
         <v>77</v>
@@ -1818,10 +1833,10 @@
         <v>70</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H49" s="6">
         <f t="shared" si="1"/>
@@ -1830,10 +1845,10 @@
     </row>
     <row r="50" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C50" s="3">
         <v>101</v>
@@ -1853,10 +1868,10 @@
     </row>
     <row r="51" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C51" s="4">
         <v>102</v>
@@ -1876,10 +1891,10 @@
     </row>
     <row r="52" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C52" s="3">
         <v>103</v>
@@ -1899,10 +1914,10 @@
     </row>
     <row r="53" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C53" s="3">
         <v>104</v>
@@ -1922,10 +1937,10 @@
     </row>
     <row r="54" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C54" s="3">
         <v>105</v>
@@ -1937,10 +1952,10 @@
         <v>28</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>12</v>
+        <v>62</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H54" s="6">
         <f t="shared" si="1"/>
@@ -1949,10 +1964,10 @@
     </row>
     <row r="55" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C55" s="4">
         <v>106</v>
@@ -1972,10 +1987,10 @@
     </row>
     <row r="56" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C56" s="3">
         <v>107</v>
@@ -1995,10 +2010,10 @@
     </row>
     <row r="57" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C57" s="3">
         <v>108</v>
@@ -2018,10 +2033,10 @@
     </row>
     <row r="58" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C58" s="3">
         <v>109</v>
@@ -2041,10 +2056,10 @@
     </row>
     <row r="59" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C59" s="4">
         <v>110</v>
@@ -2064,10 +2079,10 @@
     </row>
     <row r="60" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C60" s="3">
         <v>111</v>
@@ -2087,10 +2102,10 @@
     </row>
     <row r="61" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C61" s="3">
         <v>112</v>
@@ -2110,10 +2125,10 @@
     </row>
     <row r="62" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A62" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C62" s="3">
         <v>113</v>
@@ -2133,10 +2148,10 @@
     </row>
     <row r="63" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C63" s="4">
         <v>114</v>
@@ -2148,9 +2163,11 @@
       <c r="E63" s="3">
         <v>30</v>
       </c>
-      <c r="F63" s="5"/>
+      <c r="F63" s="5" t="s">
+        <v>63</v>
+      </c>
       <c r="G63" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H63" s="6">
         <f t="shared" si="1"/>
@@ -2159,10 +2176,10 @@
     </row>
     <row r="64" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A64" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C64" s="3">
         <v>115</v>
@@ -2182,10 +2199,10 @@
     </row>
     <row r="65" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C65" s="3">
         <v>116</v>
@@ -2205,10 +2222,10 @@
     </row>
     <row r="66" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C66" s="3">
         <v>117</v>
@@ -2228,10 +2245,10 @@
     </row>
     <row r="67" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C67" s="4">
         <v>118</v>
@@ -2251,10 +2268,10 @@
     </row>
     <row r="68" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A68" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C68" s="3">
         <v>119</v>
@@ -2274,10 +2291,10 @@
     </row>
     <row r="69" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A69" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C69" s="3">
         <v>120</v>
@@ -2297,10 +2314,10 @@
     </row>
     <row r="70" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A70" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C70" s="3">
         <v>121</v>
@@ -2320,10 +2337,10 @@
     </row>
     <row r="71" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A71" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C71" s="4">
         <v>122</v>
@@ -2343,10 +2360,10 @@
     </row>
     <row r="72" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A72" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C72" s="3">
         <v>123</v>
@@ -2358,10 +2375,10 @@
         <v>20</v>
       </c>
       <c r="F72" s="5" t="s">
-        <v>46</v>
+        <v>64</v>
       </c>
       <c r="G72" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H72" s="6">
         <f t="shared" si="2"/>
@@ -2370,10 +2387,10 @@
     </row>
     <row r="73" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A73" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C73" s="3">
         <v>124</v>
@@ -2393,10 +2410,10 @@
     </row>
     <row r="74" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A74" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C74" s="3">
         <v>125</v>
@@ -2416,10 +2433,10 @@
     </row>
     <row r="75" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A75" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C75" s="4">
         <v>126</v>
@@ -2439,10 +2456,10 @@
     </row>
     <row r="76" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A76" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C76" s="3">
         <v>127</v>
@@ -2462,10 +2479,10 @@
     </row>
     <row r="77" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A77" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C77" s="3">
         <v>128</v>
@@ -2485,10 +2502,10 @@
     </row>
     <row r="78" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A78" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C78" s="3">
         <v>129</v>
@@ -2508,10 +2525,10 @@
     </row>
     <row r="79" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A79" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C79" s="4">
         <v>130</v>
@@ -2531,10 +2548,10 @@
     </row>
     <row r="80" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A80" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C80" s="3">
         <v>131</v>
@@ -2554,10 +2571,10 @@
     </row>
     <row r="81" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A81" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C81" s="3">
         <v>132</v>
@@ -2569,10 +2586,10 @@
         <v>20</v>
       </c>
       <c r="F81" s="5" t="s">
-        <v>47</v>
+        <v>65</v>
       </c>
       <c r="G81" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H81" s="6">
         <f t="shared" si="2"/>
@@ -2581,10 +2598,10 @@
     </row>
     <row r="82" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A82" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C82" s="3">
         <v>133</v>
@@ -2604,10 +2621,10 @@
     </row>
     <row r="83" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A83" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C83" s="4">
         <v>134</v>
@@ -2627,10 +2644,10 @@
     </row>
     <row r="84" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A84" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C84" s="3">
         <v>135</v>
@@ -2650,10 +2667,10 @@
     </row>
     <row r="85" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A85" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C85" s="3">
         <v>136</v>
@@ -2673,10 +2690,10 @@
     </row>
     <row r="86" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A86" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C86" s="3">
         <v>137</v>
@@ -2696,10 +2713,10 @@
     </row>
     <row r="87" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A87" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C87" s="4">
         <v>138</v>
@@ -2719,10 +2736,10 @@
     </row>
     <row r="88" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A88" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C88" s="3">
         <v>139</v>
@@ -2742,10 +2759,10 @@
     </row>
     <row r="89" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A89" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C89" s="3">
         <v>140</v>
@@ -2765,10 +2782,10 @@
     </row>
     <row r="90" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A90" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C90" s="3">
         <v>141</v>
@@ -2780,10 +2797,10 @@
         <v>20</v>
       </c>
       <c r="F90" s="5" t="s">
-        <v>48</v>
+        <v>66</v>
       </c>
       <c r="G90" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H90" s="6">
         <f t="shared" si="2"/>
@@ -2792,10 +2809,10 @@
     </row>
     <row r="91" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A91" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C91" s="4">
         <v>142</v>
@@ -2815,10 +2832,10 @@
     </row>
     <row r="92" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A92" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C92" s="3">
         <v>143</v>
@@ -2838,10 +2855,10 @@
     </row>
     <row r="93" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A93" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C93" s="3">
         <v>144</v>
@@ -2861,10 +2878,10 @@
     </row>
     <row r="94" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A94" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C94" s="3">
         <v>145</v>
@@ -2884,10 +2901,10 @@
     </row>
     <row r="95" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A95" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C95" s="4">
         <v>146</v>
@@ -2907,10 +2924,10 @@
     </row>
     <row r="96" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A96" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C96" s="3">
         <v>147</v>
@@ -2930,10 +2947,10 @@
     </row>
     <row r="97" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A97" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C97" s="3">
         <v>148</v>
@@ -2954,10 +2971,10 @@
     </row>
     <row r="98" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A98" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C98" s="3">
         <v>149</v>
@@ -2977,10 +2994,10 @@
     </row>
     <row r="99" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A99" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C99" s="4">
         <v>150</v>
@@ -3000,10 +3017,10 @@
     </row>
     <row r="100" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A100" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C100" s="3">
         <v>28</v>
@@ -3023,10 +3040,10 @@
     </row>
     <row r="101" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A101" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C101" s="4">
         <v>27</v>
@@ -3046,10 +3063,10 @@
     </row>
     <row r="102" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A102" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C102" s="3">
         <v>26</v>
@@ -3069,10 +3086,10 @@
     </row>
     <row r="103" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A103" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C103" s="4">
         <v>25</v>
@@ -3092,10 +3109,10 @@
     </row>
     <row r="104" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A104" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C104" s="3">
         <v>24</v>
@@ -3115,10 +3132,10 @@
     </row>
     <row r="105" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A105" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C105" s="3">
         <v>23</v>
@@ -3138,10 +3155,10 @@
     </row>
     <row r="106" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A106" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C106" s="4">
         <v>22</v>
@@ -3153,10 +3170,10 @@
         <v>70</v>
       </c>
       <c r="F106" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G106" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H106" s="6">
         <f t="shared" si="3"/>
@@ -3165,10 +3182,10 @@
     </row>
     <row r="107" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A107" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C107" s="3">
         <v>21</v>
@@ -3188,10 +3205,10 @@
     </row>
     <row r="108" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A108" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C108" s="4">
         <v>20</v>
@@ -3211,10 +3228,10 @@
     </row>
     <row r="109" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A109" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C109" s="3">
         <v>19</v>
@@ -3234,10 +3251,10 @@
     </row>
     <row r="110" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A110" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C110" s="3">
         <v>18</v>
@@ -3257,10 +3274,10 @@
     </row>
     <row r="111" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A111" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C111" s="4">
         <v>17</v>
@@ -3280,10 +3297,10 @@
     </row>
     <row r="112" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A112" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C112" s="3">
         <v>16</v>
@@ -3295,10 +3312,10 @@
         <v>70</v>
       </c>
       <c r="F112" s="5" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="G112" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H112" s="6">
         <f t="shared" si="3"/>
@@ -3307,10 +3324,10 @@
     </row>
     <row r="113" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A113" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C113" s="4">
         <v>15</v>
@@ -3330,10 +3347,10 @@
     </row>
     <row r="114" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A114" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C114" s="3">
         <v>14</v>
@@ -3353,10 +3370,10 @@
     </row>
     <row r="115" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A115" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C115" s="3">
         <v>13</v>
@@ -3376,10 +3393,10 @@
     </row>
     <row r="116" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A116" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C116" s="4">
         <v>12</v>
@@ -3399,10 +3416,10 @@
     </row>
     <row r="117" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A117" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C117" s="3">
         <v>11</v>
@@ -3422,10 +3439,10 @@
     </row>
     <row r="118" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A118" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C118" s="4">
         <v>10</v>
@@ -3445,10 +3462,10 @@
     </row>
     <row r="119" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A119" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C119" s="3">
         <v>9</v>
@@ -3460,10 +3477,10 @@
         <v>45</v>
       </c>
       <c r="F119" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G119" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H119" s="6">
         <f t="shared" si="3"/>
@@ -3472,10 +3489,10 @@
     </row>
     <row r="120" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A120" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C120" s="3">
         <v>8</v>
@@ -3495,10 +3512,10 @@
     </row>
     <row r="121" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A121" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C121" s="4">
         <v>7</v>
@@ -3518,10 +3535,10 @@
     </row>
     <row r="122" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A122" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C122" s="3">
         <v>6</v>
@@ -3541,10 +3558,10 @@
     </row>
     <row r="123" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A123" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C123" s="3">
         <v>5</v>
@@ -3564,10 +3581,10 @@
     </row>
     <row r="124" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A124" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C124" s="4">
         <v>4</v>
@@ -3587,10 +3604,10 @@
     </row>
     <row r="125" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A125" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C125" s="3">
         <v>3</v>
@@ -3614,7 +3631,7 @@
         <v>Green</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C126" s="3">
         <v>2</v>
@@ -3626,10 +3643,10 @@
         <v>45</v>
       </c>
       <c r="F126" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G126" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H126" s="6">
         <f t="shared" si="3"/>
@@ -3642,7 +3659,7 @@
         <v>Green</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C127" s="4">
         <v>1</v>
@@ -3666,7 +3683,7 @@
         <v>Green</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C128" s="3">
         <v>13</v>
@@ -3690,7 +3707,7 @@
         <v>Green</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C129" s="3">
         <v>14</v>
@@ -3714,7 +3731,7 @@
         <v>Green</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C130" s="4">
         <v>15</v>
@@ -3738,7 +3755,7 @@
         <v>Green</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C131" s="3">
         <v>16</v>
@@ -3750,10 +3767,10 @@
         <v>70</v>
       </c>
       <c r="F131" s="5" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="G131" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H131" s="6">
         <f t="shared" si="5"/>
@@ -3766,7 +3783,7 @@
         <v>Green</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C132" s="4">
         <v>17</v>
@@ -3790,7 +3807,7 @@
         <v>Green</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C133" s="3">
         <v>18</v>
@@ -3814,7 +3831,7 @@
         <v>Green</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C134" s="3">
         <v>19</v>
@@ -3838,7 +3855,7 @@
         <v>Green</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C135" s="4">
         <v>20</v>
@@ -3862,7 +3879,7 @@
         <v>Green</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C136" s="3">
         <v>21</v>
@@ -3886,7 +3903,7 @@
         <v>Green</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C137" s="4">
         <v>22</v>
@@ -3898,10 +3915,10 @@
         <v>70</v>
       </c>
       <c r="F137" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G137" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H137" s="6">
         <f t="shared" si="5"/>
@@ -3914,7 +3931,7 @@
         <v>Green</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C138" s="3">
         <v>23</v>
@@ -3938,7 +3955,7 @@
         <v>Green</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C139" s="3">
         <v>24</v>
@@ -3962,7 +3979,7 @@
         <v>Green</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C140" s="4">
         <v>25</v>
@@ -3986,7 +4003,7 @@
         <v>Green</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C141" s="3">
         <v>26</v>
@@ -4010,7 +4027,7 @@
         <v>Green</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C142" s="4">
         <v>27</v>
@@ -4034,7 +4051,7 @@
         <v>Green</v>
       </c>
       <c r="B143" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C143" s="3">
         <v>28</v>
@@ -4058,7 +4075,7 @@
         <v>Green</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C144" s="3">
         <v>29</v>
@@ -4082,7 +4099,7 @@
         <v>Green</v>
       </c>
       <c r="B145" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C145" s="4">
         <v>30</v>
@@ -4106,7 +4123,7 @@
         <v>Green</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C146" s="3">
         <v>31</v>
@@ -4118,10 +4135,10 @@
         <v>30</v>
       </c>
       <c r="F146" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G146" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H146" s="6">
         <f t="shared" si="5"/>
@@ -4134,7 +4151,7 @@
         <v>Green</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C147" s="4">
         <v>32</v>
@@ -4158,7 +4175,7 @@
         <v>Green</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C148" s="3">
         <v>33</v>
@@ -4182,7 +4199,7 @@
         <v>Green</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C149" s="3">
         <v>34</v>
@@ -4206,7 +4223,7 @@
         <v>Green</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C150" s="4">
         <v>35</v>
@@ -4230,7 +4247,7 @@
         <v>Green</v>
       </c>
       <c r="B151" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C151" s="3">
         <v>36</v>
@@ -4254,7 +4271,7 @@
         <v>Green</v>
       </c>
       <c r="B152" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C152" s="3">
         <v>37</v>
@@ -4278,7 +4295,7 @@
         <v>Green</v>
       </c>
       <c r="B153" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C153" s="4">
         <v>38</v>
@@ -4302,7 +4319,7 @@
         <v>Green</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C154" s="3">
         <v>39</v>
@@ -4314,10 +4331,10 @@
         <v>30</v>
       </c>
       <c r="F154" s="5" t="s">
-        <v>48</v>
+        <v>67</v>
       </c>
       <c r="G154" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H154" s="6">
         <f t="shared" si="5"/>
@@ -4330,7 +4347,7 @@
         <v>Green</v>
       </c>
       <c r="B155" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C155" s="3">
         <v>40</v>
@@ -4354,7 +4371,7 @@
         <v>Green</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C156" s="4">
         <v>41</v>
@@ -4378,7 +4395,7 @@
         <v>Green</v>
       </c>
       <c r="B157" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C157" s="3">
         <v>42</v>
@@ -4402,7 +4419,7 @@
         <v>Green</v>
       </c>
       <c r="B158" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C158" s="3">
         <v>43</v>
@@ -4426,7 +4443,7 @@
         <v>Green</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C159" s="4">
         <v>44</v>
@@ -4450,7 +4467,7 @@
         <v>Green</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C160" s="3">
         <v>45</v>
@@ -4474,7 +4491,7 @@
         <v>Green</v>
       </c>
       <c r="B161" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C161" s="3">
         <v>46</v>
@@ -4498,7 +4515,7 @@
         <v>Green</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C162" s="4">
         <v>47</v>
@@ -4522,7 +4539,7 @@
         <v>Green</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C163" s="3">
         <v>48</v>
@@ -4534,10 +4551,10 @@
         <v>30</v>
       </c>
       <c r="F163" s="5" t="s">
-        <v>47</v>
+        <v>68</v>
       </c>
       <c r="G163" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H163" s="6">
         <f t="shared" si="6"/>
@@ -4550,7 +4567,7 @@
         <v>Green</v>
       </c>
       <c r="B164" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C164" s="3">
         <v>49</v>
@@ -4574,7 +4591,7 @@
         <v>Green</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C165" s="4">
         <v>50</v>
@@ -4598,7 +4615,7 @@
         <v>Green</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C166" s="3">
         <v>51</v>
@@ -4622,7 +4639,7 @@
         <v>Green</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C167" s="3">
         <v>52</v>
@@ -4646,7 +4663,7 @@
         <v>Green</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C168" s="4">
         <v>53</v>
@@ -4670,7 +4687,7 @@
         <v>Green</v>
       </c>
       <c r="B169" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C169" s="3">
         <v>54</v>
@@ -4694,7 +4711,7 @@
         <v>Green</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C170" s="3">
         <v>55</v>
@@ -4718,7 +4735,7 @@
         <v>Green</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C171" s="4">
         <v>56</v>
@@ -4742,7 +4759,7 @@
         <v>Green</v>
       </c>
       <c r="B172" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C172" s="3">
         <v>57</v>
@@ -4754,10 +4771,10 @@
         <v>30</v>
       </c>
       <c r="F172" s="5" t="s">
-        <v>46</v>
+        <v>69</v>
       </c>
       <c r="G172" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H172" s="6">
         <f t="shared" si="6"/>
@@ -4770,7 +4787,7 @@
         <v>Green</v>
       </c>
       <c r="B173" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C173" s="3">
         <v>58</v>
@@ -4782,7 +4799,7 @@
         <v>30</v>
       </c>
       <c r="F173" s="5" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="G173" s="3"/>
       <c r="H173" s="6">
@@ -4802,7 +4819,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{681D3D5A-AA2E-42DC-90C6-FB0A28127D18}">
   <dimension ref="A1:H106"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="G97" sqref="G97"/>
     </sheetView>
   </sheetViews>
@@ -4821,36 +4838,36 @@
   <sheetData>
     <row r="1" spans="1:8" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C2" s="7">
         <v>9</v>
@@ -4862,7 +4879,7 @@
         <v>40</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="H2" s="7">
         <f>D2*(1/(E2*1000/(60*60)))</f>
@@ -4871,10 +4888,10 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C3" s="7">
         <v>8</v>
@@ -4892,10 +4909,10 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C4" s="7">
         <v>7</v>
@@ -4907,10 +4924,10 @@
         <v>40</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H4" s="7">
         <f t="shared" ref="H4" si="0">D4*(1/(E4*1000/(60*60)))</f>
@@ -4919,10 +4936,10 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C5" s="7">
         <v>6</v>
@@ -4936,10 +4953,10 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C6" s="7">
         <v>5</v>
@@ -4953,10 +4970,10 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C7" s="7">
         <v>4</v>
@@ -4970,10 +4987,10 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C8" s="7">
         <v>3</v>
@@ -4987,10 +5004,10 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C9" s="7">
         <v>2</v>
@@ -5004,10 +5021,10 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C10" s="7">
         <v>1</v>
@@ -5021,10 +5038,10 @@
     </row>
     <row r="11" spans="1:8" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C11" s="8">
         <v>16</v>
@@ -5036,18 +5053,18 @@
         <v>40</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C12" s="10">
         <v>17</v>
@@ -5063,10 +5080,10 @@
     </row>
     <row r="13" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C13" s="8">
         <v>18</v>
@@ -5082,10 +5099,10 @@
     </row>
     <row r="14" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C14" s="8">
         <v>19</v>
@@ -5101,10 +5118,10 @@
     </row>
     <row r="15" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C15" s="10">
         <v>20</v>
@@ -5120,10 +5137,10 @@
     </row>
     <row r="16" spans="1:8" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C16" s="8">
         <v>21</v>
@@ -5135,18 +5152,18 @@
         <v>55</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C17" s="10">
         <v>22</v>
@@ -5161,10 +5178,10 @@
     </row>
     <row r="18" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C18" s="8">
         <v>23</v>
@@ -5179,10 +5196,10 @@
     </row>
     <row r="19" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C19" s="8">
         <v>24</v>
@@ -5197,10 +5214,10 @@
     </row>
     <row r="20" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C20" s="10">
         <v>25</v>
@@ -5212,18 +5229,18 @@
         <v>70</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="G20" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C21" s="8">
         <v>26</v>
@@ -5238,10 +5255,10 @@
     </row>
     <row r="22" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C22" s="10">
         <v>27</v>
@@ -5256,10 +5273,10 @@
     </row>
     <row r="23" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C23" s="8">
         <v>28</v>
@@ -5274,10 +5291,10 @@
     </row>
     <row r="24" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C24" s="8">
         <v>29</v>
@@ -5292,10 +5309,10 @@
     </row>
     <row r="25" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C25" s="10">
         <v>30</v>
@@ -5310,10 +5327,10 @@
     </row>
     <row r="26" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C26" s="8">
         <v>31</v>
@@ -5328,10 +5345,10 @@
     </row>
     <row r="27" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C27" s="10">
         <v>32</v>
@@ -5346,10 +5363,10 @@
     </row>
     <row r="28" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C28" s="8">
         <v>33</v>
@@ -5364,10 +5381,10 @@
     </row>
     <row r="29" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C29" s="8">
         <v>34</v>
@@ -5382,10 +5399,10 @@
     </row>
     <row r="30" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C30" s="10">
         <v>35</v>
@@ -5397,18 +5414,18 @@
         <v>70</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C31" s="8">
         <v>36</v>
@@ -5423,10 +5440,10 @@
     </row>
     <row r="32" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C32" s="8">
         <v>37</v>
@@ -5441,10 +5458,10 @@
     </row>
     <row r="33" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A33" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C33" s="10">
         <v>38</v>
@@ -5459,10 +5476,10 @@
     </row>
     <row r="34" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C34" s="8">
         <v>39</v>
@@ -5477,10 +5494,10 @@
     </row>
     <row r="35" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C35" s="8">
         <v>40</v>
@@ -5495,10 +5512,10 @@
     </row>
     <row r="36" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C36" s="10">
         <v>41</v>
@@ -5513,10 +5530,10 @@
     </row>
     <row r="37" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A37" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C37" s="8">
         <v>42</v>
@@ -5531,10 +5548,10 @@
     </row>
     <row r="38" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A38" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C38" s="8">
         <v>43</v>
@@ -5549,10 +5566,10 @@
     </row>
     <row r="39" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C39" s="10">
         <v>44</v>
@@ -5567,10 +5584,10 @@
     </row>
     <row r="40" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C40" s="8">
         <v>45</v>
@@ -5582,18 +5599,18 @@
         <v>70</v>
       </c>
       <c r="F40" s="9" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="G40" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A41" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C41" s="8">
         <v>46</v>
@@ -5608,10 +5625,10 @@
     </row>
     <row r="42" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C42" s="10">
         <v>47</v>
@@ -5626,10 +5643,10 @@
     </row>
     <row r="43" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A43" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C43" s="8">
         <v>48</v>
@@ -5641,18 +5658,18 @@
         <v>70</v>
       </c>
       <c r="F43" s="9" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="G43" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A44" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C44" s="8">
         <v>49</v>
@@ -5667,10 +5684,10 @@
     </row>
     <row r="45" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A45" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C45" s="10">
         <v>50</v>
@@ -5685,10 +5702,10 @@
     </row>
     <row r="46" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A46" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C46" s="8">
         <v>51</v>
@@ -5703,10 +5720,10 @@
     </row>
     <row r="47" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A47" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C47" s="8">
         <v>52</v>
@@ -5721,10 +5738,10 @@
     </row>
     <row r="48" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A48" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C48" s="10">
         <v>53</v>
@@ -5739,10 +5756,10 @@
     </row>
     <row r="49" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A49" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C49" s="8">
         <v>54</v>
@@ -5757,7 +5774,7 @@
     </row>
     <row r="50" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A50" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B50" s="8" t="s">
         <v>0</v>
@@ -5775,7 +5792,7 @@
     </row>
     <row r="51" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A51" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B51" s="8" t="s">
         <v>0</v>
@@ -5793,7 +5810,7 @@
     </row>
     <row r="52" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A52" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B52" s="8" t="s">
         <v>0</v>
@@ -5811,10 +5828,10 @@
     </row>
     <row r="53" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A53" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C53" s="8">
         <v>58</v>
@@ -5829,10 +5846,10 @@
     </row>
     <row r="54" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A54" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C54" s="10">
         <v>59</v>
@@ -5847,10 +5864,10 @@
     </row>
     <row r="55" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A55" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C55" s="8">
         <v>60</v>
@@ -5862,18 +5879,18 @@
         <v>55</v>
       </c>
       <c r="F55" s="9" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="G55" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A56" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C56" s="8">
         <v>61</v>
@@ -5888,10 +5905,10 @@
     </row>
     <row r="57" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A57" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C57" s="10">
         <v>62</v>
@@ -5906,10 +5923,10 @@
     </row>
     <row r="58" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A58" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B58" s="8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C58" s="8">
         <v>63</v>
@@ -5924,10 +5941,10 @@
     </row>
     <row r="59" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A59" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C59" s="8">
         <v>64</v>
@@ -5942,10 +5959,10 @@
     </row>
     <row r="60" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A60" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C60" s="10">
         <v>65</v>
@@ -5960,10 +5977,10 @@
     </row>
     <row r="61" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A61" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C61" s="8">
         <v>66</v>
@@ -5978,10 +5995,10 @@
     </row>
     <row r="62" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A62" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C62" s="8">
         <v>52</v>
@@ -5996,10 +6013,10 @@
     </row>
     <row r="63" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A63" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C63" s="8">
         <v>51</v>
@@ -6014,10 +6031,10 @@
     </row>
     <row r="64" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A64" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B64" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C64" s="10">
         <v>50</v>
@@ -6032,10 +6049,10 @@
     </row>
     <row r="65" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A65" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C65" s="8">
         <v>49</v>
@@ -6050,10 +6067,10 @@
     </row>
     <row r="66" spans="1:6" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A66" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B66" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C66" s="8">
         <v>48</v>
@@ -6065,15 +6082,15 @@
         <v>70</v>
       </c>
       <c r="F66" s="9" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="67" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A67" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C67" s="10">
         <v>47</v>
@@ -6088,10 +6105,10 @@
     </row>
     <row r="68" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A68" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B68" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C68" s="8">
         <v>46</v>
@@ -6106,10 +6123,10 @@
     </row>
     <row r="69" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A69" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C69" s="8">
         <v>45</v>
@@ -6121,15 +6138,15 @@
         <v>70</v>
       </c>
       <c r="F69" s="9" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="70" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A70" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B70" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C70" s="10">
         <v>44</v>
@@ -6141,15 +6158,15 @@
         <v>70</v>
       </c>
       <c r="F70" s="8" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="71" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A71" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B71" s="8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C71" s="8">
         <v>67</v>
@@ -6164,10 +6181,10 @@
     </row>
     <row r="72" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A72" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B72" s="8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C72" s="10">
         <v>68</v>
@@ -6182,10 +6199,10 @@
     </row>
     <row r="73" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A73" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B73" s="8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C73" s="8">
         <v>69</v>
@@ -6200,10 +6217,10 @@
     </row>
     <row r="74" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A74" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B74" s="8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C74" s="8">
         <v>70</v>
@@ -6218,10 +6235,10 @@
     </row>
     <row r="75" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A75" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B75" s="8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C75" s="10">
         <v>71</v>
@@ -6236,10 +6253,10 @@
     </row>
     <row r="76" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A76" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B76" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C76" s="10">
         <v>38</v>
@@ -6254,10 +6271,10 @@
     </row>
     <row r="77" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A77" s="7" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C77" s="8">
         <v>37</v>
@@ -6276,7 +6293,7 @@
         <v>Red</v>
       </c>
       <c r="B78" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C78" s="8">
         <v>36</v>
@@ -6295,7 +6312,7 @@
         <v>Red</v>
       </c>
       <c r="B79" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C79" s="10">
         <v>35</v>
@@ -6307,7 +6324,7 @@
         <v>70</v>
       </c>
       <c r="F79" s="9" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="80" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -6316,7 +6333,7 @@
         <v>Red</v>
       </c>
       <c r="B80" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C80" s="8">
         <v>34</v>
@@ -6335,7 +6352,7 @@
         <v>Red</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C81" s="8">
         <v>33</v>
@@ -6354,7 +6371,7 @@
         <v>Red</v>
       </c>
       <c r="B82" s="8" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C82" s="8">
         <v>72</v>
@@ -6373,7 +6390,7 @@
         <v>Red</v>
       </c>
       <c r="B83" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C83" s="8">
         <v>73</v>
@@ -6392,7 +6409,7 @@
         <v>Red</v>
       </c>
       <c r="B84" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C84" s="10">
         <v>74</v>
@@ -6411,7 +6428,7 @@
         <v>Red</v>
       </c>
       <c r="B85" s="8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C85" s="8">
         <v>75</v>
@@ -6430,7 +6447,7 @@
         <v>Red</v>
       </c>
       <c r="B86" s="8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C86" s="8">
         <v>76</v>
@@ -6449,7 +6466,7 @@
         <v>Red</v>
       </c>
       <c r="B87" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C87" s="10">
         <v>27</v>
@@ -6468,7 +6485,7 @@
         <v>Red</v>
       </c>
       <c r="B88" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C88" s="8">
         <v>26</v>
@@ -6487,7 +6504,7 @@
         <v>Red</v>
       </c>
       <c r="B89" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C89" s="10">
         <v>25</v>
@@ -6499,7 +6516,7 @@
         <v>70</v>
       </c>
       <c r="F89" s="9" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="90" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -6508,7 +6525,7 @@
         <v>Red</v>
       </c>
       <c r="B90" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C90" s="8">
         <v>24</v>
@@ -6527,7 +6544,7 @@
         <v>Red</v>
       </c>
       <c r="B91" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C91" s="8">
         <v>23</v>
@@ -6546,7 +6563,7 @@
         <v>Red</v>
       </c>
       <c r="B92" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C92" s="10">
         <v>22</v>
@@ -6565,7 +6582,7 @@
         <v>Red</v>
       </c>
       <c r="B93" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C93" s="8">
         <v>21</v>
@@ -6577,7 +6594,7 @@
         <v>55</v>
       </c>
       <c r="F93" s="9" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="94" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -6586,7 +6603,7 @@
         <v>Red</v>
       </c>
       <c r="B94" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C94" s="10">
         <v>20</v>
@@ -6605,7 +6622,7 @@
         <v>Red</v>
       </c>
       <c r="B95" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C95" s="8">
         <v>19</v>
@@ -6624,7 +6641,7 @@
         <v>Red</v>
       </c>
       <c r="B96" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C96" s="8">
         <v>18</v>
@@ -6643,7 +6660,7 @@
         <v>Red</v>
       </c>
       <c r="B97" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C97" s="10">
         <v>17</v>
@@ -6662,7 +6679,7 @@
         <v>Red</v>
       </c>
       <c r="B98" s="8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C98" s="8">
         <v>16</v>
@@ -6674,15 +6691,15 @@
         <v>40</v>
       </c>
       <c r="F98" s="9" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="99" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A99" s="8" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B99" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C99" s="10">
         <v>1</v>
@@ -6701,7 +6718,7 @@
         <v>Red</v>
       </c>
       <c r="B100" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C100" s="8">
         <v>2</v>
@@ -6720,7 +6737,7 @@
         <v>Red</v>
       </c>
       <c r="B101" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C101" s="8">
         <v>3</v>
@@ -6739,7 +6756,7 @@
         <v>Red</v>
       </c>
       <c r="B102" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C102" s="10">
         <v>4</v>
@@ -6758,7 +6775,7 @@
         <v>Red</v>
       </c>
       <c r="B103" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C103" s="8">
         <v>5</v>
@@ -6777,7 +6794,7 @@
         <v>Red</v>
       </c>
       <c r="B104" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C104" s="8">
         <v>6</v>
@@ -6796,7 +6813,7 @@
         <v>Red</v>
       </c>
       <c r="B105" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C105" s="10">
         <v>7</v>
@@ -6808,7 +6825,7 @@
         <v>40</v>
       </c>
       <c r="F105" s="9" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="106" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -6817,7 +6834,7 @@
         <v>Red</v>
       </c>
       <c r="B106" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C106" s="8">
         <v>8</v>
@@ -6829,7 +6846,7 @@
         <v>40</v>
       </c>
       <c r="F106" s="8" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>